<commit_message>
docs update, added coe description
</commit_message>
<xml_diff>
--- a/docs/specs.xlsx
+++ b/docs/specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keajacm\Documents\repositories\CPU_8b\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34708AD9-47B9-4B2B-A546-D68D092BD8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEA4CDC-05D1-4E65-BA38-4CA513011911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3E307697-5078-4AAF-8DD1-2E810E75D562}"/>
   </bookViews>
@@ -38,137 +38,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="134">
-  <si>
-    <t>opcode</t>
-  </si>
-  <si>
-    <t>purpose</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>store to ram</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
   <si>
     <t>d(ram) = r</t>
   </si>
   <si>
-    <t>load immediate</t>
-  </si>
-  <si>
     <t>d &lt;- k</t>
   </si>
   <si>
-    <t>load from ram</t>
-  </si>
-  <si>
     <t>d = r(ram)</t>
   </si>
   <si>
-    <t>NOP</t>
-  </si>
-  <si>
     <t>000000xxxxxxxxxx</t>
   </si>
   <si>
-    <t>jump</t>
-  </si>
-  <si>
-    <t>branch if zero?</t>
-  </si>
-  <si>
     <t>if Z then PC &lt;- p</t>
   </si>
   <si>
-    <t>branch if carry?</t>
-  </si>
-  <si>
     <t>if C then PC &lt;- p</t>
   </si>
   <si>
-    <t>LSL</t>
-  </si>
-  <si>
-    <t>*make sure you can use the same d and r if desired</t>
-  </si>
-  <si>
-    <t>ROL</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>ROR</t>
-  </si>
-  <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t>addc</t>
-  </si>
-  <si>
-    <t>sub</t>
-  </si>
-  <si>
-    <t>subc</t>
-  </si>
-  <si>
-    <t>compare</t>
-  </si>
-  <si>
-    <t>1s complement</t>
-  </si>
-  <si>
     <t>d = !r</t>
   </si>
   <si>
-    <t>move/copy</t>
-  </si>
-  <si>
     <t>d = r</t>
   </si>
   <si>
-    <t>AND</t>
-  </si>
-  <si>
     <t>d = d &amp;&amp; r</t>
   </si>
   <si>
-    <t>OR</t>
-  </si>
-  <si>
     <t>d = d || r</t>
   </si>
   <si>
     <t>d = d ^ r</t>
   </si>
   <si>
-    <t>increment</t>
-  </si>
-  <si>
-    <t>2s complement</t>
-  </si>
-  <si>
-    <t>no operation</t>
-  </si>
-  <si>
     <t>d = r + 1</t>
   </si>
   <si>
     <t>d = (!r) + 1</t>
   </si>
   <si>
-    <t>decrement</t>
-  </si>
-  <si>
     <t>d = r - 1</t>
   </si>
   <si>
@@ -205,9 +115,6 @@
     <t>F9</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -235,30 +142,12 @@
     <t>x</t>
   </si>
   <si>
-    <t>XOR</t>
-  </si>
-  <si>
     <t>x = don’t care</t>
   </si>
   <si>
-    <t>gpr</t>
-  </si>
-  <si>
-    <t>ram</t>
-  </si>
-  <si>
     <t>all on port must be in or out</t>
   </si>
   <si>
-    <t>if 01 then mask next 4 bits for ALU operation</t>
-  </si>
-  <si>
-    <t>if 1, then only a 2 bit opcode</t>
-  </si>
-  <si>
-    <t>CZ</t>
-  </si>
-  <si>
     <t>op decoder</t>
   </si>
   <si>
@@ -310,24 +199,9 @@
     <t>I/O for PMOD JA</t>
   </si>
   <si>
-    <t>PC &lt;= p</t>
-  </si>
-  <si>
     <t>101ddddddddrrrrr</t>
   </si>
   <si>
-    <t>clear C</t>
-  </si>
-  <si>
-    <t>set C</t>
-  </si>
-  <si>
-    <t>clear Z</t>
-  </si>
-  <si>
-    <t>set Z</t>
-  </si>
-  <si>
     <t>000100xxxxxxxxxx</t>
   </si>
   <si>
@@ -340,21 +214,12 @@
     <t>000111xxxxxxxxxx</t>
   </si>
   <si>
-    <t>clear I</t>
-  </si>
-  <si>
-    <t>set I</t>
-  </si>
-  <si>
     <t>000010xxxxxxxxxx</t>
   </si>
   <si>
     <t>000011xxxxxxxxxx</t>
   </si>
   <si>
-    <t>no interrputs used rn</t>
-  </si>
-  <si>
     <t>100rrrrrrrrddddd</t>
   </si>
   <si>
@@ -424,9 +289,6 @@
     <t>xxxxxxbbbbbaaaaa</t>
   </si>
   <si>
-    <t>d = d, Z if d = r else !Z</t>
-  </si>
-  <si>
     <t>timer stuff (TBD)</t>
   </si>
   <si>
@@ -439,7 +301,145 @@
     <t>sreg</t>
   </si>
   <si>
-    <t>xxxx xxZC</t>
+    <t>*currently not implemented</t>
+  </si>
+  <si>
+    <t>xxxx xIZC</t>
+  </si>
+  <si>
+    <t>ST: store to ram</t>
+  </si>
+  <si>
+    <t>LD: load from ram</t>
+  </si>
+  <si>
+    <t>LDI: load immediate</t>
+  </si>
+  <si>
+    <t>MV: move/copy</t>
+  </si>
+  <si>
+    <t>LSL: logical shift left</t>
+  </si>
+  <si>
+    <t>ROL: rotate left</t>
+  </si>
+  <si>
+    <t>LSR: logical shift right</t>
+  </si>
+  <si>
+    <t>ROR: rotate right</t>
+  </si>
+  <si>
+    <t>SUBC: subtract with carry</t>
+  </si>
+  <si>
+    <t>SUB: subtract</t>
+  </si>
+  <si>
+    <t>ADDC: add with carry</t>
+  </si>
+  <si>
+    <t>ADD: add</t>
+  </si>
+  <si>
+    <t>ONEC: 1s complement</t>
+  </si>
+  <si>
+    <t>TWOC: 2s complement</t>
+  </si>
+  <si>
+    <t>AND: bitwise and</t>
+  </si>
+  <si>
+    <t>OR: bitwise or</t>
+  </si>
+  <si>
+    <t>XOR: bitwise xor</t>
+  </si>
+  <si>
+    <t>INC: increment</t>
+  </si>
+  <si>
+    <t>DEC: decrement</t>
+  </si>
+  <si>
+    <t>COMP: compare registers</t>
+  </si>
+  <si>
+    <t>Z = (d == r)</t>
+  </si>
+  <si>
+    <t>NOP: no operation</t>
+  </si>
+  <si>
+    <t>CLC: clear C</t>
+  </si>
+  <si>
+    <t>SEC: set C</t>
+  </si>
+  <si>
+    <t>CLZ: clear Z</t>
+  </si>
+  <si>
+    <t>SEZ: set Z</t>
+  </si>
+  <si>
+    <t>CLI: clear I</t>
+  </si>
+  <si>
+    <t>SEI: set I</t>
+  </si>
+  <si>
+    <t>JUMP: jump instruction</t>
+  </si>
+  <si>
+    <t>BRZ: branch if zero</t>
+  </si>
+  <si>
+    <t>BRC: branch if carry</t>
+  </si>
+  <si>
+    <t>PC = p</t>
+  </si>
+  <si>
+    <t>OPCODE NAME/DESCRIPTION</t>
+  </si>
+  <si>
+    <t>OPCODE</t>
+  </si>
+  <si>
+    <t>DETAILS</t>
+  </si>
+  <si>
+    <t>UTILIZES</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>GPR, C, Z</t>
+  </si>
+  <si>
+    <t>RAM, GPR</t>
+  </si>
+  <si>
+    <t>GPR, Z</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>PC, Z</t>
+  </si>
+  <si>
+    <t>PC, C</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -512,6 +512,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,16 +830,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F324A3-08EA-4FBA-B549-7C9553005D70}">
-  <dimension ref="A2:G53"/>
+  <dimension ref="A2:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="44.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
@@ -844,576 +847,578 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="C9" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>70</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="1" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="1" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
@@ -1458,85 +1463,85 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1563,23 +1568,23 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -1587,10 +1592,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1598,26 +1603,26 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C9" s="7" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>